<commit_message>
Fixed data numbers for 0.15.9
</commit_message>
<xml_diff>
--- a/costs.xlsx
+++ b/costs.xlsx
@@ -1,20 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\andrewgu\factorioplanner\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="10785"/>
+    <workbookView xWindow="6420" yWindow="1470" windowWidth="11175" windowHeight="13440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$75</definedName>
+  </definedNames>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -158,7 +156,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -496,7 +494,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -506,14 +504,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66:XFD66"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.9296875" customWidth="1"/>
-    <col min="2" max="2" width="20.86328125" customWidth="1"/>
+    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
@@ -529,65 +527,65 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C4">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
       <c r="C5">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6">
         <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -595,10 +593,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -606,21 +604,21 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -628,10 +626,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -639,54 +637,54 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="C12">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="B13" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -694,10 +692,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -708,7 +706,7 @@
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -716,21 +714,21 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -738,120 +736,120 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C21">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B22" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C22">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B23" t="s">
         <v>14</v>
       </c>
       <c r="C23">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B24" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="C24">
-        <v>2</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C25">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="C26">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="B27" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C27">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B28" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B29" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C29">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B30" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C30">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B31" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -859,24 +857,24 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B32" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C32">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B33" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C33">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.45">
@@ -887,114 +885,114 @@
         <v>5</v>
       </c>
       <c r="C34">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B35" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="C35">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B36" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C36">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="B37" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C37">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="B38" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C38">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B39" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C39">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B40" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="C40">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B41" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="C41">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B42" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="C42">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B43" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="C43">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="B44" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="C44">
         <v>1</v>
@@ -1002,10 +1000,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="B45" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -1013,43 +1011,43 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="B46" t="s">
         <v>14</v>
       </c>
       <c r="C46">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="B47" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C47">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="B48" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C48">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B49" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C49">
         <v>1</v>
@@ -1057,109 +1055,109 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B50" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C50">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B51" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="C51">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B52" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C52">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B53" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C53">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B54" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C54">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B55" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C55">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="B56" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C56">
-        <v>40</v>
+        <v>2</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="B57" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="C57">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="B58" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="C58">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="B59" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="C59">
         <v>1</v>
@@ -1167,10 +1165,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="B60" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C60">
         <v>1</v>
@@ -1178,32 +1176,32 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B61" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C61">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B62" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="C62">
-        <v>2</v>
+        <v>15</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B63" t="s">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="C63">
         <v>5</v>
@@ -1211,137 +1209,142 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B64" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C64">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B65" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="C65">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="B66" t="s">
-        <v>39</v>
+        <v>5</v>
       </c>
       <c r="C66">
-        <v>0.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B67" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="C67">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B68" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C68">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B69" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="C69">
-        <v>5</v>
+        <v>100</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="B70" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C70">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="B71" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C71">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B72" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C72">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B73" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="C73">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B74" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C74">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B75" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="C75">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C75">
+    <sortState ref="A2:C75">
+      <sortCondition ref="A1:A75"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed throughput calculation weirdness on sulfur
</commit_message>
<xml_diff>
--- a/costs.xlsx
+++ b/costs.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\andrewgu\factorioplanner\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="6420" yWindow="1470" windowWidth="11175" windowHeight="13440"/>
   </bookViews>
@@ -156,7 +161,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -494,7 +499,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -508,10 +513,10 @@
       <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.86328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">

</xml_diff>